<commit_message>
added units and format column
</commit_message>
<xml_diff>
--- a/data-raw/labels.xlsx
+++ b/data-raw/labels.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="15"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="vehicle_type" sheetId="1" state="visible" r:id="rId2"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="69">
   <si>
     <t xml:space="preserve">from</t>
   </si>
@@ -54,7 +54,7 @@
     <t xml:space="preserve">Kleinwagen</t>
   </si>
   <si>
-    <t xml:space="preserve">small_car</t>
+    <t xml:space="preserve">small</t>
   </si>
   <si>
     <t xml:space="preserve">Luxusklasse</t>
@@ -144,6 +144,12 @@
     <t xml:space="preserve">Wasserstoff / Elektro</t>
   </si>
   <si>
+    <t xml:space="preserve">filter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">long</t>
+  </si>
+  <si>
     <t xml:space="preserve">Small car</t>
   </si>
   <si>
@@ -159,6 +165,15 @@
     <t xml:space="preserve">Luxury car or sports coupé</t>
   </si>
   <si>
+    <t xml:space="preserve">short</t>
+  </si>
+  <si>
+    <t xml:space="preserve">archs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">revert</t>
+  </si>
+  <si>
     <t xml:space="preserve">Gasoline</t>
   </si>
   <si>
@@ -171,16 +186,46 @@
     <t xml:space="preserve">Plug-in hybrid</t>
   </si>
   <si>
+    <t xml:space="preserve">unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">km</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHF/month</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHF/km</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 CHF/month</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12 CHF/month</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 CHF/h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 CHF/h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.8 CHF/km</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.2 CHF/km</t>
+  </si>
+  <si>
     <t xml:space="preserve">1 km or less</t>
   </si>
   <si>
-    <t xml:space="preserve">more than 1 km</t>
-  </si>
-  <si>
-    <t xml:space="preserve">up to 25 km/h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">up to 45 km/h</t>
+    <t xml:space="preserve">More than 1 km</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Up to 25 km/h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Up to 45 km/h</t>
   </si>
   <si>
     <t xml:space="preserve">GA</t>
@@ -198,7 +243,7 @@
     <t xml:space="preserve">2-5 zones</t>
   </si>
   <si>
-    <t xml:space="preserve">included</t>
+    <t xml:space="preserve">Included</t>
   </si>
 </sst>
 </file>
@@ -302,10 +347,10 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J16" activeCellId="0" sqref="J16"/>
+      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.83"/>
   </cols>
@@ -440,13 +485,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -458,18 +503,23 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="n">
-        <v>0.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="n">
-        <v>1.3</v>
+      <c r="B4" s="0" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -488,13 +538,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -506,18 +556,23 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>44</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>45</v>
+      <c r="B4" s="0" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -536,13 +591,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -554,18 +609,23 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>46</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>47</v>
+      <c r="B4" s="0" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -584,13 +644,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -599,21 +659,35 @@
       <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="0" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="n">
-        <v>0.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B4" s="0" t="n">
         <v>1.3</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -632,13 +706,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F28" activeCellId="0" sqref="F28"/>
+      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -650,26 +724,31 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>48</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>50</v>
+      <c r="B5" s="0" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -688,13 +767,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -706,18 +785,23 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>51</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>52</v>
+      <c r="B4" s="0" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -736,13 +820,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -754,18 +838,20 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>53</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
         <v>2</v>
-      </c>
-      <c r="B3" s="0" t="n">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -784,13 +870,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -799,21 +885,35 @@
       <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="0" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="n">
-        <v>0.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B4" s="0" t="n">
         <v>1.3</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -832,13 +932,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G42" activeCellId="0" sqref="G42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -847,21 +947,35 @@
       <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="0" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="n">
-        <v>0.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B4" s="0" t="n">
         <v>1.3</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -883,10 +997,13 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.93"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -978,13 +1095,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G20" activeCellId="0" sqref="G20"/>
+      <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.1"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -993,45 +1113,244 @@
       <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="0" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>35</v>
+        <v>0</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>37</v>
+        <v>2</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>38</v>
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B7" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
         <v>39</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1050,13 +1369,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+      <selection pane="topLeft" activeCell="G25" activeCellId="0" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -1065,45 +1384,244 @@
       <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="0" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>40</v>
+        <v>0</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>23</v>
+        <v>45</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>41</v>
+        <v>23</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>42</v>
+        <v>46</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B7" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="0" t="s">
         <v>43</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1122,13 +1640,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="D37" activeCellId="0" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -1137,21 +1655,35 @@
       <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="0" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="n">
-        <v>0.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B4" s="0" t="n">
         <v>1.3</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1170,13 +1702,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L35" activeCellId="0" sqref="L35"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -1185,21 +1717,35 @@
       <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="0" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="n">
-        <v>0.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B4" s="0" t="n">
         <v>1.3</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1218,13 +1764,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -1233,21 +1779,35 @@
       <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="0" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="n">
-        <v>0.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B4" s="0" t="n">
         <v>1.3</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1266,13 +1826,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -1284,18 +1844,23 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="n">
-        <v>0.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="n">
-        <v>1.3</v>
+      <c r="B4" s="0" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1314,13 +1879,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -1332,18 +1897,23 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="n">
-        <v>0.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="n">
-        <v>1.3</v>
+      <c r="B4" s="0" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>